<commit_message>
Update attendance on 20 march
</commit_message>
<xml_diff>
--- a/Poseschaemost_i_rezultaty_testov.xlsx
+++ b/Poseschaemost_i_rezultaty_testov.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="19420" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="19420" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="84">
   <si>
     <t>9 класс</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Сычёв</t>
+  </si>
+  <si>
+    <t>Дорохова        9 Е</t>
   </si>
 </sst>
 </file>
@@ -640,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,7 +654,7 @@
     <col min="1" max="1" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -697,8 +700,11 @@
       <c r="O1" s="1">
         <v>43537</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" s="1">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -729,8 +735,11 @@
       <c r="N2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -738,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -767,7 +776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -775,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -786,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -797,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -805,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -842,8 +851,11 @@
       <c r="O9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -851,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -862,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -873,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -887,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -895,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -903,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -914,15 +926,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>62</v>
       </c>
       <c r="N17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -932,29 +947,32 @@
       <c r="O18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="O19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="O20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="O21" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>